<commit_message>
sidequest, mais pas que
</commit_message>
<xml_diff>
--- a/output/repas.xlsx
+++ b/output/repas.xlsx
@@ -1,42 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="repas 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="repas 2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="repas 3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="repas 4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="repas 5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="repas 6" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="repas 7" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="repas 8" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="repas 9" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="repas 10" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="repas 11" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="repas 12" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="repas 13" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="repas 14" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="repas 15" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="repas 16" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="repas 17" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="repas 18" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="repas 19" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="repas 20" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="repas 21" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="repas 22" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="repas 23" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="repas 24" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="repas 25" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="repas 26" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="repas 27" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="repas 28" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="repas 29" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="repas 30" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 10" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 11" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 12" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 13" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 14" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 15" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 16" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 17" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 18" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 19" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 20" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 21" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 22" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 23" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 24" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 25" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 26" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 27" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 28" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 29" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 30" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 31" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 32" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 33" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 34" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 35" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 36" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 37" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 38" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 39" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 40" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 41" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="repas 42" sheetId="42" state="visible" r:id="rId42"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -477,51 +489,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cassava</t>
+          <t>Potatoes</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90.96505564116499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dark Chocolate</t>
+          <t>Wine</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.246926995423044e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Soymilk</t>
+          <t>Groundnuts</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>984.3855398420667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.803835486009933</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tomatoes</t>
+          <t>Root Vegetables</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.975333961919182e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +543,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8.300401631110114e-11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -572,7 +584,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>157.5130590232161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -588,17 +600,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cheese</t>
+          <t>Peas</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>84.18741205582613</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Palm Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -618,7 +630,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Berries &amp; Grapes</t>
+          <t>Bananas</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -663,17 +675,17 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>167.1950245941377</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wine</t>
+          <t>Beet Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.738577123222495e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -683,37 +695,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>41.74289913607614</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sunflower Oil</t>
+          <t>Rapeseed Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.677280221992363e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Brassicas</t>
+          <t>Onions &amp; Leeks</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>285.1541361722156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other Fruit</t>
+          <t>Berries &amp; Grapes</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7.320236657767964e-11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -750,17 +762,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oatmeal</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>160.1302752963581</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wine</t>
+          <t>Dark Chocolate</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -770,7 +782,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pig Meat</t>
+          <t>Tofu</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -780,27 +792,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Soybean Oil</t>
+          <t>Palm Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.5293803268536</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Other Vegetables</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>618.3647108942546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other Fruit</t>
+          <t>Apples</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -845,37 +857,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>247.2026118723566</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dark Chocolate</t>
+          <t>Cane Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.241628749288793e-08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lamb &amp; Mutton</t>
+          <t>Nuts</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>109.4323112047459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sunflower Oil</t>
+          <t>Olive Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.16939265236276</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -885,17 +897,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.970974494724942e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other Fruit</t>
+          <t>Berries &amp; Grapes</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.24065202555812e-09</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -932,17 +944,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wheat &amp; Rye (Bread)</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>246.1999872410644</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wine</t>
+          <t>Coffee</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -952,27 +964,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Crustaceans (farmed)</t>
+          <t>Poultry Meat</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>151.5211055210923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Sunflower Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.85260805580263</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tomatoes</t>
+          <t>Onions &amp; Leeks</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -982,7 +994,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Citrus Fruit</t>
+          <t>Other Fruit</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1023,17 +1035,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Potatoes</t>
+          <t>Maize (Meal)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>538.6616794325497</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Coffee</t>
+          <t>Barley (Beer)</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1043,37 +1055,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tofu</t>
+          <t>Bovine Meat (beef herd)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>312.9190616165504</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Sunflower Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.53268172674868</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Root Vegetables</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.183479932690392e-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Berries &amp; Grapes</t>
+          <t>Bananas</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1114,17 +1126,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Maize (Meal)</t>
+          <t>Cassava</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>158.4833849774245</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Barley (Beer)</t>
+          <t>Dark Chocolate</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1134,11 +1146,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Fish (farmed)</t>
+          <t>Other Pulses</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>197.7862798235786</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1148,13 +1160,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.61227752924772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Root Vegetables</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1164,7 +1176,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Citrus Fruit</t>
+          <t>Bananas</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1205,11 +1217,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Cassava</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.775934719616389e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1225,41 +1237,41 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Milk</t>
+          <t>Crustaceans (farmed)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>784.3506053233177</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sunflower Oil</t>
+          <t>Palm Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.333867301366521e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Onions &amp; Leeks</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1088.267560730181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Citrus Fruit</t>
+          <t>Berries &amp; Grapes</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.59699151618857e-11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1300,47 +1312,47 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.686044963923201e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wine</t>
+          <t>Cane Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.992723123169621e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Other Pulses</t>
+          <t>Pig Meat</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>155.8088636303524</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sunflower Oil</t>
+          <t>Palm Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.45194499302679</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Onions &amp; Leeks</t>
+          <t>Root Vegetables</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.714072074663603e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1350,7 +1362,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7.240052869562105e-12</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1387,51 +1399,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oatmeal</t>
+          <t>Wheat &amp; Rye (Bread)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>193.0661830823952</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wine</t>
+          <t>Cane Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.096604594633126e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Eggs</t>
+          <t>Crustaceans (farmed)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>29.97664342559968</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Olive Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.675677476475469</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Onions &amp; Leeks</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.419923777850682e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1441,7 +1453,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.836798641012212e-11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1478,7 +1490,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cassava</t>
+          <t>Wheat &amp; Rye (Bread)</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1488,7 +1500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Coffee</t>
+          <t>Dark Chocolate</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1498,37 +1510,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Fish (farmed)</t>
+          <t>Cheese</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>223.4564809629762</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Sunflower Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.36514205696508</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Onions &amp; Leeks</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1513.08043113101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bananas</t>
+          <t>Other Fruit</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1569,17 +1581,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wheat &amp; Rye (Bread)</t>
+          <t>Cassava</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>206.8051282032456</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Barley (Beer)</t>
+          <t>Cane Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1593,13 +1605,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>64.62660256291295</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sunflower Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1619,7 +1631,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Citrus Fruit</t>
+          <t>Apples</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1660,17 +1672,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Potatoes</t>
+          <t>Maize (Meal)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>841.4648405342131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Barley (Beer)</t>
+          <t>Wine</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1680,27 +1692,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Crustaceans (farmed)</t>
+          <t>Nuts</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>223.8423312790833</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Palm Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>22.77928115669937</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tomatoes</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1710,7 +1722,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Berries &amp; Grapes</t>
+          <t>Citrus Fruit</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1751,11 +1763,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oatmeal</t>
+          <t>Wheat &amp; Rye (Bread)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>183.9284786904136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1771,37 +1783,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Milk</t>
+          <t>Peas</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>142.6711800391596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6.972912064821356</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Brassicas</t>
+          <t>Other Vegetables</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.452330458773647e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Apples</t>
+          <t>Berries &amp; Grapes</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1842,7 +1854,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cassava</t>
+          <t>Wheat &amp; Rye (Bread)</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1852,7 +1864,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dark Chocolate</t>
+          <t>Coffee</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1862,7 +1874,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Groundnuts</t>
+          <t>Poultry Meat</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1872,7 +1884,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Palm Oil</t>
+          <t>Olive Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1892,7 +1904,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Berries &amp; Grapes</t>
+          <t>Apples</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1933,17 +1945,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Potatoes</t>
+          <t>Oatmeal</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>362.2354143238133</v>
+        <v>129.7644303200523</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Barley (Beer)</t>
+          <t>Cane Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1953,7 +1965,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bovine Meat (beef herd)</t>
+          <t>Milk</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1963,11 +1975,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Soybean Oil</t>
+          <t>Sunflower Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.02266076787945</v>
+        <v>10.15340039557505</v>
       </c>
     </row>
     <row r="6">
@@ -1977,13 +1989,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2034.441673555265</v>
+        <v>501.1029040805954</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bananas</t>
+          <t>Apples</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2028,13 +2040,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>471.94278985486</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Beet Sugar</t>
+          <t>Cane Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2044,17 +2056,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pig Meat</t>
+          <t>Soymilk</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>96.87246738660909</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2064,21 +2076,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tomatoes</t>
+          <t>Root Vegetables</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1887.771159411899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Apples</t>
+          <t>Citrus Fruit</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.662694030889076e-15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2115,31 +2127,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Maize (Meal)</t>
+          <t>Potatoes</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>67.41118181495786</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Beet Sugar</t>
+          <t>Barley (Beer)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.613997075437847e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nuts</t>
+          <t>Other Pulses</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.671225001581493e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2149,27 +2161,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19.51643115778445</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Other Vegetables</t>
+          <t>Onions &amp; Leeks</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2043.957909071294</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Other Fruit</t>
+          <t>Berries &amp; Grapes</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.036013614184225e-10</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2206,7 +2218,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Potatoes</t>
+          <t>Wheat &amp; Rye (Bread)</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -2216,7 +2228,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Beet Sugar</t>
+          <t>Dark Chocolate</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2226,27 +2238,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Other Pulses</t>
+          <t>Tofu</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>155.8088636361752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sunflower Oil</t>
+          <t>Olive Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.45194499333291</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Root Vegetables</t>
+          <t>Onions &amp; Leeks</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2256,7 +2268,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Berries &amp; Grapes</t>
+          <t>Bananas</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2297,61 +2309,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wheat &amp; Rye (Bread)</t>
+          <t>Maize (Meal)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.931522196697511e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dark Chocolate</t>
+          <t>Coffee</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7.531948955498772e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Peas</t>
+          <t>Cheese</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>152.3464444447404</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Olive Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.85840289923888</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tomatoes</t>
+          <t>Onions &amp; Leeks</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.135319312037714e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Apples</t>
+          <t>Berries &amp; Grapes</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.279465757245481e-11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2388,17 +2400,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oatmeal</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>160.1302752963939</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Coffee</t>
+          <t>Wine</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2408,7 +2420,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Fish (farmed)</t>
+          <t>Groundnuts</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2418,11 +2430,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Olive Oil</t>
+          <t>Rapeseed Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.52938032556631</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2432,7 +2444,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>618.36471089427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2479,61 +2491,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Potatoes</t>
+          <t>Maize (Meal)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>362.2354147281644</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wine</t>
+          <t>Cane Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.016609661068059e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Poultry Meat</t>
+          <t>Groundnuts</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.630313508188937e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Olive Oil</t>
+          <t>Rapeseed Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.02266077634938</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Other Vegetables</t>
+          <t>Onions &amp; Leeks</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2034.441668882113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Berries &amp; Grapes</t>
+          <t>Citrus Fruit</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.112205115161004e-11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2570,11 +2582,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oatmeal</t>
+          <t>Maize (Meal)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>193.0661830849152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2590,41 +2602,860 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Eggs</t>
+          <t>Pig Meat</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>29.9766434202488</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Palm Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.67567747636986</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Onions &amp; Leeks</t>
+          <t>Tomatoes</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.210222922033708e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Other Fruit</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Potatoes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Soymilk</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sunflower Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Other Vegetables</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Bananas</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.362089704084867e-10</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Wine</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Crustaceans (farmed)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Rapeseed Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tomatoes</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Apples</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cassava</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cane Sugar</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Peas</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Palm Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Brassicas</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bananas</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Oatmeal</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Wine</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Eggs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Olive Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Brassicas</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other Fruit</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Maize (Meal)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Barley (Beer)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Eggs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Olive Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Brassicas</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Apples</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cassava</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Dark Chocolate</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bovine Meat (dairy herd)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Palm Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Onions &amp; Leeks</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Citrus Fruit</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cassava</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cane Sugar</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Groundnuts</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Soybean Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Other Vegetables</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other Fruit</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Maize (Meal)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>82.91751158954685</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Wine</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.839789547375403e-07</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tofu</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>253.8131593701851</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Soybean Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7.460149687684861</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tomatoes</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2.590982148831245e-07</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Apples</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.48765593621647e-07</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Wheat &amp; Rye (Bread)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Peas</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sunflower Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Other Vegetables</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other Fruit</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2661,51 +3492,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Potatoes</t>
+          <t>Oatmeal</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>825.6263103992193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cane Sugar</t>
+          <t>Beet Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.956155297446961e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Eggs</t>
+          <t>Bovine Meat (beef herd)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>186.4418498570436</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rapeseed Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.274563432440115e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Other Vegetables</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.406665735773579e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2715,7 +3546,280 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.748023413804984e-10</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Potatoes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beet Sugar</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Lamb &amp; Mutton</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Olive Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Brassicas</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Citrus Fruit</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Maize (Meal)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cane Sugar</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cheese</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Soybean Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Other Vegetables</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bananas</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrédient</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantités</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Potatoes</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Wine</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Nuts</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Soybean Oil</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Root Vegetables</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Apples</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2772,41 +3876,41 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Crustaceans (farmed)</t>
+          <t>Fish (farmed)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>219.5509268784576</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Soybean Oil</t>
+          <t>Olive Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.36744561109128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Root Vegetables</t>
+          <t>Other Vegetables</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1540.275990234634</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bananas</t>
+          <t>Other Fruit</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.968817050012576e-09</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2843,17 +3947,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cassava</t>
+          <t>Wheat &amp; Rye (Bread)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>484.281732468417</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Coffee</t>
+          <t>Dark Chocolate</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2863,27 +3967,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Poultry Meat</t>
+          <t>Fish (farmed)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>243.2472715375697</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sunflower Oil</t>
+          <t>Palm Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.427568784293206</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Brassicas</t>
+          <t>Other Vegetables</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2934,17 +4038,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Potatoes</t>
+          <t>Wheat &amp; Rye (Bread)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>362.2354142758927</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dark Chocolate</t>
+          <t>Barley (Beer)</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2954,7 +4058,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bovine Meat (beef herd)</t>
+          <t>Fish (farmed)</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2968,23 +4072,23 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20.02266080677937</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Other Vegetables</t>
+          <t>Root Vegetables</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2034.441672889517</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bananas</t>
+          <t>Apples</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3025,21 +4129,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oatmeal</t>
+          <t>Maize (Meal)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>193.6413283661641</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Barley (Beer)</t>
+          <t>Beet Sugar</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.879745304813301e-11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -3049,37 +4153,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>13.18134984866722</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Palm Oil</t>
+          <t>Soybean Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.137331008096274</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Root Vegetables</t>
+          <t>Brassicas</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.077241464451159e-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Apples</t>
+          <t>Citrus Fruit</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.775426213679967e-11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3116,11 +4220,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cassava</t>
+          <t>Oatmeal</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33.17269608070222</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -3136,7 +4240,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cheese</t>
+          <t>Bovine Meat (dairy herd)</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -3146,11 +4250,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Palm Oil</t>
+          <t>Olive Oil</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.07356706626141</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -3160,13 +4264,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3397.939573526993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Apples</t>
+          <t>Berries &amp; Grapes</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>